<commit_message>
Function to edit status of tasks added
</commit_message>
<xml_diff>
--- a/Chore Tracker.xlsx
+++ b/Chore Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp/Documents/GitHub/chore-tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3E2C62-84A8-6B45-850C-A4748436796C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648682BD-3ABC-2B4F-861B-EEC722FDB42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" xr2:uid="{4ABEB36C-A057-0140-B9A6-5DF66DAE2C03}"/>
   </bookViews>
@@ -36,22 +36,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Test 1</t>
-  </si>
-  <si>
-    <t>Test 2</t>
-  </si>
-  <si>
-    <t>Test 3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Ganden</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>Laundry</t>
+  </si>
+  <si>
+    <t>Forge signatures</t>
+  </si>
+  <si>
+    <t>Snapper</t>
+  </si>
+  <si>
+    <t>Gapper</t>
+  </si>
+  <si>
+    <t>Siege</t>
+  </si>
+  <si>
+    <t>Impact</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -61,6 +88,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,8 +120,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,93 +438,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B095F122-EC47-1D4D-9C3C-8F5811B5D886}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="B1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>92</v>
-      </c>
-      <c r="B2">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>56</v>
-      </c>
-      <c r="C2">
-        <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <f t="shared" ref="A3:C6" ca="1" si="0">RANDBETWEEN(1,100)</f>
-        <v>43</v>
-      </c>
-      <c r="B3">
-        <f t="shared" ca="1" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ca="1" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <f t="shared" ca="1" si="0"/>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45266</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>45278</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>11</v>
-      </c>
-      <c r="B4">
-        <f t="shared" ca="1" si="0"/>
-        <v>98</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ca="1" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <f t="shared" ca="1" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B5">
-        <f t="shared" ca="1" si="0"/>
-        <v>98</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ca="1" si="0"/>
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <f t="shared" ca="1" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <f t="shared" ca="1" si="0"/>
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed file upload for tasks
</commit_message>
<xml_diff>
--- a/Chore Tracker.xlsx
+++ b/Chore Tracker.xlsx
@@ -1,40 +1,106 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp/Documents/GitHub/chore-tracker/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE6AAA6-6A2D-5047-83DB-7B737F981AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Sample Task 1</t>
+  </si>
+  <si>
+    <t>Sample Task 2</t>
+  </si>
+  <si>
+    <t>Sample Task 3</t>
+  </si>
+  <si>
+    <t>Sample Task 4</t>
+  </si>
+  <si>
+    <t>Sample Task 5</t>
+  </si>
+  <si>
+    <t>Sample Task 6</t>
+  </si>
+  <si>
+    <t>Person 1</t>
+  </si>
+  <si>
+    <t>Person 2</t>
+  </si>
+  <si>
+    <t>Person 3</t>
+  </si>
+  <si>
+    <t>Person 4</t>
+  </si>
+  <si>
+    <t>Person 5</t>
+  </si>
+  <si>
+    <t>Person 6</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,94 +115,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -424,126 +440,115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Assignee</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Due Date</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Laundry</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Ganden</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
         <v>45266</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Forge signatures</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Marco</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="n">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
         <v>45278</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Snapper</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45279</v>
+      </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Gapper</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>45280</v>
+      </c>
       <c r="D5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Siege</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2">
+        <v>45281</v>
+      </c>
       <c r="D6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Impact</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2">
+        <v>45282</v>
+      </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates ALL status to false
</commit_message>
<xml_diff>
--- a/Chore Tracker.xlsx
+++ b/Chore Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp/Documents/GitHub/chore-tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A9D685F-C640-6F44-B643-C227EC9AB31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1386A86F-9AB4-474E-8EBB-510CA735C5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Task</t>
   </si>
@@ -34,49 +34,34 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Sample Task 1</t>
-  </si>
-  <si>
-    <t>Sample Task 2</t>
-  </si>
-  <si>
-    <t>Sample Task 3</t>
-  </si>
-  <si>
-    <t>Sample Task 4</t>
-  </si>
-  <si>
-    <t>Sample Task 5</t>
-  </si>
-  <si>
     <t>Sample Task 6</t>
   </si>
   <si>
-    <t>Person 1</t>
-  </si>
-  <si>
-    <t>Person 2</t>
-  </si>
-  <si>
-    <t>Person 3</t>
-  </si>
-  <si>
-    <t>Person 4</t>
-  </si>
-  <si>
-    <t>Person 5</t>
-  </si>
-  <si>
-    <t>Person 6</t>
+    <t>Laundry</t>
+  </si>
+  <si>
+    <t>Gapper</t>
+  </si>
+  <si>
+    <t>#########</t>
+  </si>
+  <si>
+    <t>Siege</t>
+  </si>
+  <si>
+    <t>Warb</t>
+  </si>
+  <si>
+    <t>Dishes</t>
+  </si>
+  <si>
+    <t>Floor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,13 +71,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,7 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -114,31 +101,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,7 +413,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -465,13 +434,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45266</v>
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -479,13 +448,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45278</v>
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -493,13 +462,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2">
-        <v>45279</v>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -507,48 +476,48 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2">
-        <v>45280</v>
-      </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2">
-        <v>45281</v>
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2">
-        <v>45282</v>
+      <c r="C7" t="s">
+        <v>7</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Task progress 2 (#4)
* Fixed changing status of tasks

* Updates ALL status to false
</commit_message>
<xml_diff>
--- a/Chore Tracker.xlsx
+++ b/Chore Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp/Documents/GitHub/chore-tracker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A9D685F-C640-6F44-B643-C227EC9AB31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1386A86F-9AB4-474E-8EBB-510CA735C5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Task</t>
   </si>
@@ -34,49 +34,34 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Sample Task 1</t>
-  </si>
-  <si>
-    <t>Sample Task 2</t>
-  </si>
-  <si>
-    <t>Sample Task 3</t>
-  </si>
-  <si>
-    <t>Sample Task 4</t>
-  </si>
-  <si>
-    <t>Sample Task 5</t>
-  </si>
-  <si>
     <t>Sample Task 6</t>
   </si>
   <si>
-    <t>Person 1</t>
-  </si>
-  <si>
-    <t>Person 2</t>
-  </si>
-  <si>
-    <t>Person 3</t>
-  </si>
-  <si>
-    <t>Person 4</t>
-  </si>
-  <si>
-    <t>Person 5</t>
-  </si>
-  <si>
-    <t>Person 6</t>
+    <t>Laundry</t>
+  </si>
+  <si>
+    <t>Gapper</t>
+  </si>
+  <si>
+    <t>#########</t>
+  </si>
+  <si>
+    <t>Siege</t>
+  </si>
+  <si>
+    <t>Warb</t>
+  </si>
+  <si>
+    <t>Dishes</t>
+  </si>
+  <si>
+    <t>Floor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,13 +71,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -106,7 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -114,31 +101,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,7 +413,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -465,13 +434,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45266</v>
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -479,13 +448,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45278</v>
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -493,13 +462,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2">
-        <v>45279</v>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -507,48 +476,48 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2">
-        <v>45280</v>
-      </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2">
-        <v>45281</v>
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2">
-        <v>45282</v>
+      <c r="C7" t="s">
+        <v>7</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>